<commit_message>
Final version of scrum temp
</commit_message>
<xml_diff>
--- a/scrum_temp team 7.xlsx
+++ b/scrum_temp team 7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\git\Team7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6533654D-18B0-4227-B74D-F80069488144}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2FED88-5759-4B2C-A779-196A28B4DDC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="504" windowWidth="28800" windowHeight="16260" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="504" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guide" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="147">
   <si>
     <t>Responsible</t>
   </si>
@@ -195,12 +195,6 @@
     <t>As an admin, I am able to add, read, edit and remove election machine questions.</t>
   </si>
   <si>
-    <t>As a candidate I can modify my answers</t>
-  </si>
-  <si>
-    <t>As a candidate I can answer the questions</t>
-  </si>
-  <si>
     <t>SUMMARY</t>
   </si>
   <si>
@@ -295,15 +289,6 @@
   </si>
   <si>
     <t>Create javadoc</t>
-  </si>
-  <si>
-    <t>Coding UI</t>
-  </si>
-  <si>
-    <t>Update candidates answers to database</t>
-  </si>
-  <si>
-    <t>Add candidates answers to database</t>
   </si>
   <si>
     <t xml:space="preserve">Spring Planning </t>
@@ -1657,6 +1642,10 @@
     <xf numFmtId="0" fontId="19" fillId="12" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1676,12 +1665,39 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1693,6 +1709,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1722,38 +1739,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4577,8 +4562,8 @@
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4589,8 +4574,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="100"/>
-      <c r="B1" s="100"/>
+      <c r="A1" s="102"/>
+      <c r="B1" s="102"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4613,7 +4598,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="101" t="s">
+      <c r="A3" s="103" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -4627,32 +4612,32 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="100"/>
+      <c r="A4" s="102"/>
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="102" t="s">
+      <c r="C4" s="104" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="102" t="s">
+      <c r="D4" s="104" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="100"/>
+      <c r="A5" s="102"/>
       <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
     </row>
     <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="100"/>
+      <c r="A6" s="102"/>
       <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="102"/>
     </row>
     <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
@@ -4672,7 +4657,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="101" t="s">
+      <c r="A9" s="103" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -4686,32 +4671,32 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="100"/>
+      <c r="A10" s="102"/>
       <c r="B10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="102" t="s">
+      <c r="C10" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="102" t="s">
+      <c r="D10" s="104" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="100"/>
+      <c r="A11" s="102"/>
       <c r="B11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="100"/>
-      <c r="D11" s="100"/>
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
     </row>
     <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="100"/>
+      <c r="A12" s="102"/>
       <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
+      <c r="C12" s="102"/>
+      <c r="D12" s="102"/>
     </row>
     <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
@@ -4728,7 +4713,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="99" t="s">
+      <c r="A15" s="101" t="s">
         <v>29</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -4742,16 +4727,16 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="100"/>
+      <c r="A16" s="102"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="100"/>
+      <c r="A17" s="102"/>
     </row>
     <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="100"/>
+      <c r="A18" s="102"/>
     </row>
     <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="100"/>
+      <c r="A19" s="102"/>
     </row>
     <row r="20" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
@@ -4795,17 +4780,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="105" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
       <c r="D1" s="8"/>
-      <c r="E1" s="105" t="s">
+      <c r="E1" s="107" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="106"/>
-      <c r="G1" s="107"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="109"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
@@ -4849,7 +4834,7 @@
     </row>
     <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B4" s="12">
         <v>2</v>
@@ -4877,7 +4862,7 @@
     </row>
     <row r="6" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B6" s="12">
         <v>3</v>
@@ -4960,251 +4945,251 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="20"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="110" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="20"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="143" t="s">
+      <c r="C2" s="113" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="21" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="111"/>
+      <c r="B3" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="142" t="s">
+      <c r="C3" s="114"/>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="112"/>
+      <c r="B4" s="23" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="138"/>
-      <c r="B3" s="22" t="s">
+      <c r="C4" s="115"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="122" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="119" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="111"/>
+      <c r="B6" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="114"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="112"/>
+      <c r="B7" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="115"/>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="122" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="119" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="111"/>
+      <c r="B9" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="114"/>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="112"/>
+      <c r="B10" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="115"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="122" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="111"/>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="139"/>
-      <c r="B4" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="141"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="137" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="108" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="138"/>
-      <c r="B6" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="111"/>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="139"/>
-      <c r="B7" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="141"/>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="137" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="28" t="s">
+      <c r="B11" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" s="116" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="111"/>
+      <c r="B12" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="117"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="112"/>
+      <c r="B13" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" s="118"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="122" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="108" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="138"/>
-      <c r="B9" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="111"/>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="139"/>
-      <c r="B10" s="27" t="s">
+      <c r="C14" s="119" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="111"/>
+      <c r="B15" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="114"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="111"/>
+      <c r="B16" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="141"/>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="137" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="C11" s="145" t="s">
+      <c r="C16" s="114"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="111"/>
+      <c r="B17" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="114"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="111"/>
+      <c r="B18" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="114"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="111"/>
+      <c r="B19" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="114"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="112"/>
+      <c r="B20" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="115"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="122" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="120" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="121"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="111"/>
+      <c r="B22" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="100" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="111"/>
+      <c r="B23" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="111"/>
+      <c r="B24" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="111"/>
+      <c r="B25" s="29" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="138"/>
-      <c r="B12" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="135"/>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="139"/>
-      <c r="B13" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="C13" s="136"/>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="137" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="108" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="138"/>
-      <c r="B15" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="111"/>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="138"/>
-      <c r="B16" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="111"/>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="138"/>
-      <c r="B17" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="111"/>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="138"/>
-      <c r="B18" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="111"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="138"/>
-      <c r="B19" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="111"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="139"/>
-      <c r="B20" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="141"/>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="137" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="110" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" s="140"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="138"/>
-      <c r="B22" s="29" t="s">
+      <c r="C25" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="144" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="138"/>
-      <c r="B23" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="138"/>
-      <c r="B24" s="29" t="s">
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="111"/>
+      <c r="B26" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="138"/>
-      <c r="B25" s="29" t="s">
+      <c r="C26" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="111"/>
+      <c r="B27" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="138"/>
-      <c r="B26" s="29" t="s">
+      <c r="C27" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="111"/>
+      <c r="B28" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="138"/>
-      <c r="B27" s="29" t="s">
+      <c r="C28" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="111"/>
+      <c r="B29" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="138"/>
-      <c r="B28" s="29" t="s">
+      <c r="C29" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="112"/>
+      <c r="B30" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="138"/>
-      <c r="B29" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="139"/>
-      <c r="B30" s="29" t="s">
-        <v>76</v>
-      </c>
       <c r="C30" s="30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -5250,47 +5235,47 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5303,63 +5288,63 @@
       <c r="E4" s="38"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="114" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" s="115"/>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="116"/>
+      <c r="A5" s="125" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="126"/>
+      <c r="C5" s="126"/>
+      <c r="D5" s="126"/>
+      <c r="E5" s="127"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="109"/>
-      <c r="B6" s="104"/>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="113"/>
+      <c r="A6" s="128"/>
+      <c r="B6" s="106"/>
+      <c r="C6" s="106"/>
+      <c r="D6" s="106"/>
+      <c r="E6" s="124"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="117" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" s="118"/>
-      <c r="C7" s="118"/>
-      <c r="D7" s="118"/>
-      <c r="E7" s="119"/>
+      <c r="A7" s="129" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="130"/>
+      <c r="C7" s="130"/>
+      <c r="D7" s="130"/>
+      <c r="E7" s="131"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="34" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5374,33 +5359,33 @@
       <c r="G11" s="40"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="114" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="115"/>
-      <c r="C12" s="115"/>
-      <c r="D12" s="115"/>
-      <c r="E12" s="116"/>
+      <c r="A12" s="125" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="126"/>
+      <c r="C12" s="126"/>
+      <c r="D12" s="126"/>
+      <c r="E12" s="127"/>
       <c r="F12" s="41"/>
       <c r="G12" s="40"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="109"/>
-      <c r="B13" s="104"/>
-      <c r="C13" s="104"/>
-      <c r="D13" s="104"/>
-      <c r="E13" s="113"/>
+      <c r="A13" s="128"/>
+      <c r="B13" s="106"/>
+      <c r="C13" s="106"/>
+      <c r="D13" s="106"/>
+      <c r="E13" s="124"/>
       <c r="F13" s="41"/>
       <c r="G13" s="40"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="112" t="s">
-        <v>94</v>
-      </c>
-      <c r="B14" s="104"/>
-      <c r="C14" s="104"/>
-      <c r="D14" s="104"/>
-      <c r="E14" s="113"/>
+      <c r="A14" s="123" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="106"/>
+      <c r="C14" s="106"/>
+      <c r="D14" s="106"/>
+      <c r="E14" s="124"/>
       <c r="F14" s="39"/>
       <c r="G14" s="40"/>
     </row>
@@ -5415,38 +5400,38 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="43" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F16" s="39"/>
       <c r="G16" s="40"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="35" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F17" s="39"/>
       <c r="G17" s="40"/>
@@ -5462,32 +5447,32 @@
       <c r="G18" s="40"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="114" t="s">
-        <v>97</v>
-      </c>
-      <c r="B19" s="115"/>
-      <c r="C19" s="115"/>
-      <c r="D19" s="115"/>
-      <c r="E19" s="116"/>
+      <c r="A19" s="125" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="126"/>
+      <c r="C19" s="126"/>
+      <c r="D19" s="126"/>
+      <c r="E19" s="127"/>
       <c r="F19" s="41"/>
       <c r="G19" s="40"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="109"/>
-      <c r="B20" s="104"/>
-      <c r="C20" s="104"/>
-      <c r="D20" s="104"/>
-      <c r="E20" s="113"/>
+      <c r="A20" s="128"/>
+      <c r="B20" s="106"/>
+      <c r="C20" s="106"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="124"/>
       <c r="F20" s="41"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="112" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" s="104"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="104"/>
-      <c r="E21" s="113"/>
+      <c r="A21" s="123" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="106"/>
+      <c r="C21" s="106"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="124"/>
       <c r="F21" s="39"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6504,7 +6489,7 @@
   <dimension ref="A1:G996"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6518,182 +6503,182 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="46" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C2" s="48" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E2" s="49" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F2" s="50" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G2" s="50" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="51" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="53"/>
       <c r="E3" s="54" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F3" s="55" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G3" s="56"/>
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="57" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B4" s="58" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4" s="59"/>
       <c r="E4" s="54" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F4" s="56" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G4" s="59"/>
     </row>
     <row r="5" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="57" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" s="59"/>
       <c r="E5" s="54" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F5" s="56" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G5" s="59"/>
     </row>
     <row r="6" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="57" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B6" s="61" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" s="59"/>
       <c r="E6" s="54" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F6" s="56" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G6" s="59"/>
     </row>
     <row r="7" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="62" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B7" s="63" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7" s="59"/>
       <c r="E7" s="54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F7" s="56" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G7" s="59"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="64" t="s">
-        <v>110</v>
-      </c>
-      <c r="B8" s="134" t="s">
-        <v>52</v>
+        <v>105</v>
+      </c>
+      <c r="B8" s="99" t="s">
+        <v>50</v>
       </c>
       <c r="C8" s="60"/>
       <c r="E8" s="54" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F8" s="56" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G8" s="59"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E9" s="54" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F9" s="56" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G9" s="59"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E10" s="54" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F10" s="56" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G10" s="59"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="45" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B11" s="45" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E11" s="54" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F11" s="56" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G11" s="59"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="48" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B12" s="66" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E12" s="54" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F12" s="56" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G12" s="59"/>
     </row>
@@ -6702,25 +6687,25 @@
         <v>42</v>
       </c>
       <c r="B13" s="68" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C13" s="53" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E13" s="65" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F13" s="56" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G13" s="59"/>
     </row>
     <row r="14" spans="1:7" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="67" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B14" s="69" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" s="59"/>
     </row>
@@ -7750,58 +7735,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="120" t="s">
-        <v>115</v>
-      </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121"/>
-      <c r="I1" s="121"/>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="121"/>
-      <c r="O1" s="121"/>
-      <c r="P1" s="121"/>
-      <c r="Q1" s="121"/>
-      <c r="R1" s="121"/>
-      <c r="S1" s="122"/>
+      <c r="A1" s="132" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="133"/>
+      <c r="N1" s="133"/>
+      <c r="O1" s="133"/>
+      <c r="P1" s="133"/>
+      <c r="Q1" s="133"/>
+      <c r="R1" s="133"/>
+      <c r="S1" s="134"/>
     </row>
     <row r="2" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="71" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="71" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="71" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="G2" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="71" t="s">
+      <c r="H2" s="71" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="71" t="s">
+      <c r="I2" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="E2" s="71" t="s">
+      <c r="J2" s="72" t="s">
         <v>120</v>
-      </c>
-      <c r="F2" s="71" t="s">
-        <v>121</v>
-      </c>
-      <c r="G2" s="71" t="s">
-        <v>122</v>
-      </c>
-      <c r="H2" s="71" t="s">
-        <v>123</v>
-      </c>
-      <c r="I2" s="71" t="s">
-        <v>124</v>
-      </c>
-      <c r="J2" s="72" t="s">
-        <v>125</v>
       </c>
       <c r="L2" s="73"/>
       <c r="M2" s="73"/>
@@ -7818,22 +7803,22 @@
       <c r="C3" s="74"/>
       <c r="D3" s="74"/>
       <c r="E3" s="74" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F3" s="74" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G3" s="74" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="H3" s="74" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="I3" s="74" t="s">
-        <v>126</v>
-      </c>
-      <c r="J3" s="123" t="s">
-        <v>127</v>
+        <v>121</v>
+      </c>
+      <c r="J3" s="135" t="s">
+        <v>122</v>
       </c>
       <c r="L3" s="73"/>
       <c r="M3" s="73"/>
@@ -7846,14 +7831,14 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="75" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B4" s="75"/>
       <c r="C4" s="75" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="75" t="s">
         <v>46</v>
-      </c>
-      <c r="D4" s="75" t="s">
-        <v>48</v>
       </c>
       <c r="E4" s="76">
         <v>2</v>
@@ -7862,7 +7847,7 @@
       <c r="G4" s="77"/>
       <c r="H4" s="77"/>
       <c r="I4" s="77"/>
-      <c r="J4" s="100"/>
+      <c r="J4" s="102"/>
       <c r="K4" s="78"/>
       <c r="L4" s="79"/>
       <c r="M4" s="79"/>
@@ -7882,14 +7867,14 @@
     </row>
     <row r="5" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="80" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B5" s="81"/>
       <c r="C5" s="80" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="80" t="s">
         <v>46</v>
-      </c>
-      <c r="D5" s="80" t="s">
-        <v>48</v>
       </c>
       <c r="E5" s="76">
         <v>2</v>
@@ -7900,7 +7885,7 @@
       <c r="G5" s="77"/>
       <c r="H5" s="77"/>
       <c r="I5" s="77"/>
-      <c r="J5" s="100"/>
+      <c r="J5" s="102"/>
       <c r="L5" s="73"/>
       <c r="M5" s="73"/>
       <c r="N5" s="73"/>
@@ -7916,7 +7901,7 @@
       </c>
       <c r="B6" s="85"/>
       <c r="C6" s="83" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="74"/>
       <c r="E6" s="74"/>
@@ -7924,7 +7909,7 @@
       <c r="G6" s="74"/>
       <c r="H6" s="74"/>
       <c r="I6" s="74"/>
-      <c r="J6" s="100"/>
+      <c r="J6" s="102"/>
       <c r="K6" s="73"/>
       <c r="L6" s="73"/>
       <c r="M6" s="73"/>
@@ -7937,12 +7922,12 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="80" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" s="80"/>
       <c r="C7" s="80"/>
       <c r="D7" s="84" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E7" s="76">
         <v>3</v>
@@ -7951,7 +7936,7 @@
       <c r="G7" s="77"/>
       <c r="H7" s="77"/>
       <c r="I7" s="77"/>
-      <c r="J7" s="100"/>
+      <c r="J7" s="102"/>
       <c r="K7" s="73"/>
       <c r="L7" s="73"/>
       <c r="M7" s="73"/>
@@ -7964,12 +7949,12 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="80" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B8" s="80"/>
       <c r="C8" s="80"/>
       <c r="D8" s="84" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E8" s="77"/>
       <c r="F8" s="76">
@@ -7978,7 +7963,7 @@
       <c r="G8" s="77"/>
       <c r="H8" s="77"/>
       <c r="I8" s="77"/>
-      <c r="J8" s="100"/>
+      <c r="J8" s="102"/>
       <c r="K8" s="73"/>
       <c r="L8" s="73"/>
       <c r="M8" s="73"/>
@@ -7991,12 +7976,12 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="80" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B9" s="80"/>
       <c r="C9" s="80"/>
       <c r="D9" s="84" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E9" s="77"/>
       <c r="F9" s="77"/>
@@ -8009,7 +7994,7 @@
       <c r="I9" s="76">
         <v>5</v>
       </c>
-      <c r="J9" s="100"/>
+      <c r="J9" s="102"/>
       <c r="K9" s="73"/>
       <c r="L9" s="73"/>
       <c r="M9" s="73"/>
@@ -8022,12 +8007,12 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="80" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B10" s="80"/>
       <c r="C10" s="80"/>
       <c r="D10" s="84" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E10" s="77"/>
       <c r="F10" s="77"/>
@@ -8040,7 +8025,7 @@
       <c r="I10" s="76">
         <v>4</v>
       </c>
-      <c r="J10" s="100"/>
+      <c r="J10" s="102"/>
       <c r="K10" s="73"/>
       <c r="L10" s="73"/>
       <c r="M10" s="73"/>
@@ -8053,12 +8038,12 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="80" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B11" s="80"/>
       <c r="C11" s="80"/>
       <c r="D11" s="84" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E11" s="77"/>
       <c r="F11" s="77"/>
@@ -8067,7 +8052,7 @@
       <c r="I11" s="76">
         <v>5</v>
       </c>
-      <c r="J11" s="100"/>
+      <c r="J11" s="102"/>
       <c r="K11" s="73"/>
       <c r="L11" s="73"/>
       <c r="M11" s="73"/>
@@ -8080,11 +8065,11 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="85" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B12" s="85"/>
       <c r="C12" s="83" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" s="74"/>
       <c r="E12" s="74"/>
@@ -8092,7 +8077,7 @@
       <c r="G12" s="74"/>
       <c r="H12" s="74"/>
       <c r="I12" s="74"/>
-      <c r="J12" s="100"/>
+      <c r="J12" s="102"/>
       <c r="K12" s="73"/>
       <c r="L12" s="73"/>
       <c r="M12" s="73"/>
@@ -8105,12 +8090,12 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="84" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B13" s="80"/>
       <c r="C13" s="80"/>
       <c r="D13" s="80" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E13" s="77"/>
       <c r="F13" s="76">
@@ -8119,7 +8104,7 @@
       <c r="G13" s="77"/>
       <c r="H13" s="77"/>
       <c r="I13" s="77"/>
-      <c r="J13" s="100"/>
+      <c r="J13" s="102"/>
       <c r="K13" s="73"/>
       <c r="L13" s="73"/>
       <c r="M13" s="73"/>
@@ -8136,7 +8121,7 @@
       </c>
       <c r="B14" s="85"/>
       <c r="C14" s="83" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D14" s="74"/>
       <c r="E14" s="74"/>
@@ -8144,7 +8129,7 @@
       <c r="G14" s="74"/>
       <c r="H14" s="74"/>
       <c r="I14" s="74"/>
-      <c r="J14" s="100"/>
+      <c r="J14" s="102"/>
       <c r="K14" s="73"/>
       <c r="L14" s="73"/>
       <c r="M14" s="73"/>
@@ -8157,12 +8142,12 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="80" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B15" s="80"/>
       <c r="C15" s="80"/>
       <c r="D15" s="84" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E15" s="77"/>
       <c r="F15" s="77"/>
@@ -8171,7 +8156,7 @@
         <v>3</v>
       </c>
       <c r="I15" s="77"/>
-      <c r="J15" s="100"/>
+      <c r="J15" s="102"/>
       <c r="K15" s="73"/>
       <c r="L15" s="73"/>
       <c r="M15" s="73"/>
@@ -8184,12 +8169,12 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="80" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B16" s="80"/>
       <c r="C16" s="80"/>
       <c r="D16" s="84" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E16" s="77"/>
       <c r="F16" s="77"/>
@@ -8198,7 +8183,7 @@
       <c r="I16" s="76">
         <v>2</v>
       </c>
-      <c r="J16" s="100"/>
+      <c r="J16" s="102"/>
       <c r="K16" s="73"/>
       <c r="L16" s="73"/>
       <c r="M16" s="73"/>
@@ -8211,11 +8196,11 @@
     </row>
     <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="85" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B17" s="85"/>
       <c r="C17" s="83" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17" s="74"/>
       <c r="E17" s="74"/>
@@ -8223,7 +8208,7 @@
       <c r="G17" s="74"/>
       <c r="H17" s="74"/>
       <c r="I17" s="74"/>
-      <c r="J17" s="100"/>
+      <c r="J17" s="102"/>
       <c r="K17" s="73"/>
       <c r="L17" s="73"/>
       <c r="M17" s="73"/>
@@ -8236,12 +8221,12 @@
     </row>
     <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="80" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B18" s="80"/>
       <c r="C18" s="80"/>
       <c r="D18" s="80" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E18" s="77"/>
       <c r="F18" s="77"/>
@@ -8250,7 +8235,7 @@
       </c>
       <c r="H18" s="77"/>
       <c r="I18" s="77"/>
-      <c r="J18" s="100"/>
+      <c r="J18" s="102"/>
       <c r="K18" s="73"/>
       <c r="L18" s="73"/>
       <c r="M18" s="73"/>
@@ -8263,11 +8248,11 @@
     </row>
     <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="80" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C19" s="80"/>
       <c r="D19" s="80" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E19" s="77"/>
       <c r="F19" s="77"/>
@@ -8276,7 +8261,7 @@
       </c>
       <c r="H19" s="77"/>
       <c r="I19" s="77"/>
-      <c r="J19" s="100"/>
+      <c r="J19" s="102"/>
       <c r="K19" s="73"/>
       <c r="L19" s="73"/>
       <c r="M19" s="73"/>
@@ -8289,12 +8274,12 @@
     </row>
     <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="80" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B20" s="80"/>
       <c r="C20" s="80"/>
       <c r="D20" s="84" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E20" s="77"/>
       <c r="F20" s="77"/>
@@ -8303,7 +8288,7 @@
       <c r="I20" s="76">
         <v>1</v>
       </c>
-      <c r="J20" s="100"/>
+      <c r="J20" s="102"/>
       <c r="K20" s="73"/>
       <c r="L20" s="73"/>
       <c r="M20" s="73"/>
@@ -8316,12 +8301,12 @@
     </row>
     <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="80" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B21" s="80"/>
       <c r="C21" s="80"/>
       <c r="D21" s="80" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E21" s="77"/>
       <c r="F21" s="77"/>
@@ -8330,48 +8315,48 @@
       </c>
       <c r="H21" s="77"/>
       <c r="I21" s="77"/>
-      <c r="J21" s="100"/>
+      <c r="J21" s="102"/>
     </row>
     <row r="22" spans="1:19" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="80" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B22" s="80"/>
       <c r="C22" s="80"/>
       <c r="D22" s="80" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E22" s="77"/>
       <c r="F22" s="77"/>
       <c r="G22" s="77"/>
       <c r="H22" s="77"/>
       <c r="I22" s="77"/>
-      <c r="J22" s="100"/>
+      <c r="J22" s="102"/>
     </row>
     <row r="23" spans="1:19" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="80" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B23" s="86"/>
       <c r="C23" s="80"/>
       <c r="D23" s="80" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E23" s="77"/>
       <c r="F23" s="77"/>
       <c r="G23" s="77"/>
       <c r="H23" s="77"/>
       <c r="I23" s="77"/>
-      <c r="J23" s="100"/>
+      <c r="J23" s="102"/>
     </row>
     <row r="24" spans="1:19" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="80" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B24" s="80"/>
       <c r="C24" s="80"/>
       <c r="D24" s="80" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E24" s="77"/>
       <c r="F24" s="77"/>
@@ -8383,7 +8368,7 @@
     </row>
     <row r="25" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="87" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B25" s="87"/>
       <c r="C25" s="87"/>
@@ -9391,7 +9376,7 @@
   <dimension ref="A1:S983"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9409,58 +9394,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="120" t="s">
-        <v>137</v>
-      </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121"/>
-      <c r="I1" s="121"/>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="121"/>
-      <c r="O1" s="121"/>
-      <c r="P1" s="121"/>
-      <c r="Q1" s="121"/>
-      <c r="R1" s="121"/>
-      <c r="S1" s="122"/>
+      <c r="A1" s="132" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="133"/>
+      <c r="N1" s="133"/>
+      <c r="O1" s="133"/>
+      <c r="P1" s="133"/>
+      <c r="Q1" s="133"/>
+      <c r="R1" s="133"/>
+      <c r="S1" s="134"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="71" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="71" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="71" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="G2" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="71" t="s">
+      <c r="H2" s="71" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="71" t="s">
+      <c r="I2" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="E2" s="71" t="s">
+      <c r="J2" s="88" t="s">
         <v>120</v>
-      </c>
-      <c r="F2" s="71" t="s">
-        <v>121</v>
-      </c>
-      <c r="G2" s="71" t="s">
-        <v>122</v>
-      </c>
-      <c r="H2" s="71" t="s">
-        <v>123</v>
-      </c>
-      <c r="I2" s="71" t="s">
-        <v>124</v>
-      </c>
-      <c r="J2" s="88" t="s">
-        <v>125</v>
       </c>
       <c r="K2" s="78"/>
       <c r="L2" s="89"/>
@@ -9474,13 +9459,13 @@
     </row>
     <row r="3" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="90" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B3" s="85">
         <v>3</v>
       </c>
       <c r="C3" s="83" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="74"/>
       <c r="E3" s="74"/>
@@ -9488,8 +9473,8 @@
       <c r="G3" s="74"/>
       <c r="H3" s="74"/>
       <c r="I3" s="74"/>
-      <c r="J3" s="124" t="s">
-        <v>138</v>
+      <c r="J3" s="136" t="s">
+        <v>133</v>
       </c>
       <c r="K3" s="78"/>
       <c r="L3" s="91"/>
@@ -9503,12 +9488,12 @@
     </row>
     <row r="4" spans="1:19" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="75" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" s="86"/>
       <c r="C4" s="84"/>
       <c r="D4" s="84" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E4" s="92">
         <v>4</v>
@@ -9517,7 +9502,7 @@
       <c r="G4" s="86"/>
       <c r="H4" s="86"/>
       <c r="I4" s="86"/>
-      <c r="J4" s="125"/>
+      <c r="J4" s="137"/>
       <c r="K4" s="93"/>
       <c r="L4" s="91"/>
       <c r="M4" s="91"/>
@@ -9530,12 +9515,12 @@
     </row>
     <row r="5" spans="1:19" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="80" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B5" s="80"/>
       <c r="C5" s="84"/>
       <c r="D5" s="84" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E5" s="94"/>
       <c r="F5" s="95">
@@ -9544,7 +9529,7 @@
       <c r="G5" s="94"/>
       <c r="H5" s="94"/>
       <c r="I5" s="94"/>
-      <c r="J5" s="125"/>
+      <c r="J5" s="137"/>
       <c r="K5" s="93"/>
       <c r="L5" s="91"/>
       <c r="M5" s="91"/>
@@ -9557,12 +9542,12 @@
     </row>
     <row r="6" spans="1:19" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="80" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B6" s="80"/>
       <c r="C6" s="84"/>
       <c r="D6" s="84" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E6" s="94"/>
       <c r="F6" s="94"/>
@@ -9571,7 +9556,7 @@
       </c>
       <c r="H6" s="94"/>
       <c r="I6" s="96"/>
-      <c r="J6" s="125"/>
+      <c r="J6" s="137"/>
       <c r="K6" s="93"/>
       <c r="L6" s="91"/>
       <c r="M6" s="91"/>
@@ -9584,13 +9569,13 @@
     </row>
     <row r="7" spans="1:19" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="85" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B7" s="85">
         <v>4</v>
       </c>
       <c r="C7" s="83" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="74"/>
       <c r="E7" s="85"/>
@@ -9611,12 +9596,12 @@
     </row>
     <row r="8" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="80" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B8" s="80"/>
       <c r="C8" s="84"/>
       <c r="D8" s="84" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E8" s="94"/>
       <c r="F8" s="94"/>
@@ -9638,7 +9623,7 @@
     </row>
     <row r="9" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="87" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B9" s="87"/>
       <c r="C9" s="87"/>
@@ -10685,10 +10670,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:S1003"/>
+  <dimension ref="A1:S997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10701,60 +10686,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="120" t="s">
-        <v>141</v>
-      </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121"/>
-      <c r="I1" s="121"/>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="121"/>
-      <c r="O1" s="121"/>
-      <c r="P1" s="121"/>
-      <c r="Q1" s="121"/>
-      <c r="R1" s="121"/>
-      <c r="S1" s="122"/>
+      <c r="A1" s="132" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="133"/>
+      <c r="N1" s="133"/>
+      <c r="O1" s="133"/>
+      <c r="P1" s="133"/>
+      <c r="Q1" s="133"/>
+      <c r="R1" s="133"/>
+      <c r="S1" s="134"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="71" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="71" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="71" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="G2" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="71" t="s">
+      <c r="H2" s="71" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="71" t="s">
+      <c r="I2" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="E2" s="71" t="s">
+      <c r="J2" s="138" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="71" t="s">
-        <v>121</v>
-      </c>
-      <c r="G2" s="71" t="s">
-        <v>122</v>
-      </c>
-      <c r="H2" s="71" t="s">
-        <v>123</v>
-      </c>
-      <c r="I2" s="71" t="s">
-        <v>124</v>
-      </c>
-      <c r="J2" s="126" t="s">
-        <v>125</v>
-      </c>
-      <c r="K2" s="127"/>
+      <c r="K2" s="139"/>
       <c r="M2" s="73"/>
       <c r="N2" s="73"/>
       <c r="O2" s="73"/>
@@ -10771,7 +10756,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="83" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="74"/>
       <c r="E3" s="74"/>
@@ -10779,10 +10764,10 @@
       <c r="G3" s="74"/>
       <c r="H3" s="74"/>
       <c r="I3" s="74"/>
-      <c r="J3" s="128" t="s">
-        <v>142</v>
-      </c>
-      <c r="K3" s="129"/>
+      <c r="J3" s="140" t="s">
+        <v>137</v>
+      </c>
+      <c r="K3" s="141"/>
       <c r="L3" s="73"/>
       <c r="M3" s="73"/>
       <c r="N3" s="73"/>
@@ -10794,12 +10779,12 @@
     </row>
     <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" s="80"/>
       <c r="C4" s="80"/>
       <c r="D4" s="84" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E4" s="94"/>
       <c r="F4" s="94"/>
@@ -10808,8 +10793,8 @@
       <c r="I4" s="84">
         <v>3</v>
       </c>
-      <c r="J4" s="130"/>
-      <c r="K4" s="131"/>
+      <c r="J4" s="142"/>
+      <c r="K4" s="143"/>
       <c r="L4" s="73"/>
       <c r="M4" s="73"/>
       <c r="N4" s="73"/>
@@ -10821,12 +10806,12 @@
     </row>
     <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B5" s="80"/>
       <c r="C5" s="80"/>
       <c r="D5" s="84" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E5" s="94"/>
       <c r="F5" s="96">
@@ -10837,8 +10822,8 @@
       </c>
       <c r="H5" s="80"/>
       <c r="I5" s="80"/>
-      <c r="J5" s="130"/>
-      <c r="K5" s="131"/>
+      <c r="J5" s="142"/>
+      <c r="K5" s="143"/>
       <c r="L5" s="73"/>
       <c r="M5" s="73"/>
       <c r="N5" s="73"/>
@@ -10850,12 +10835,12 @@
     </row>
     <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" s="80"/>
       <c r="C6" s="80"/>
       <c r="D6" s="84" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E6" s="94"/>
       <c r="F6" s="94"/>
@@ -10864,8 +10849,8 @@
       <c r="I6" s="84">
         <v>3</v>
       </c>
-      <c r="J6" s="130"/>
-      <c r="K6" s="131"/>
+      <c r="J6" s="142"/>
+      <c r="K6" s="143"/>
       <c r="L6" s="73"/>
       <c r="M6" s="73"/>
       <c r="N6" s="73"/>
@@ -10877,12 +10862,12 @@
     </row>
     <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B7" s="80"/>
       <c r="C7" s="80"/>
       <c r="D7" s="84" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E7" s="94"/>
       <c r="F7" s="94"/>
@@ -10891,8 +10876,8 @@
       <c r="I7" s="84">
         <v>1</v>
       </c>
-      <c r="J7" s="130"/>
-      <c r="K7" s="131"/>
+      <c r="J7" s="142"/>
+      <c r="K7" s="143"/>
       <c r="L7" s="73"/>
       <c r="M7" s="73"/>
       <c r="N7" s="73"/>
@@ -10904,20 +10889,20 @@
     </row>
     <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B8" s="86"/>
       <c r="C8" s="80"/>
       <c r="D8" s="84" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E8" s="86"/>
       <c r="F8" s="86"/>
       <c r="G8" s="86"/>
       <c r="H8" s="75"/>
       <c r="I8" s="75"/>
-      <c r="J8" s="130"/>
-      <c r="K8" s="131"/>
+      <c r="J8" s="142"/>
+      <c r="K8" s="143"/>
       <c r="L8" s="73"/>
       <c r="M8" s="73"/>
       <c r="N8" s="73"/>
@@ -10929,12 +10914,12 @@
     </row>
     <row r="9" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" s="80"/>
       <c r="C9" s="80"/>
       <c r="D9" s="84" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E9" s="94"/>
       <c r="F9" s="94"/>
@@ -10943,8 +10928,8 @@
       <c r="I9" s="84">
         <v>4</v>
       </c>
-      <c r="J9" s="130"/>
-      <c r="K9" s="131"/>
+      <c r="J9" s="142"/>
+      <c r="K9" s="143"/>
       <c r="L9" s="73"/>
       <c r="M9" s="73"/>
       <c r="N9" s="73"/>
@@ -10956,12 +10941,12 @@
     </row>
     <row r="10" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="36" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B10" s="80"/>
       <c r="C10" s="80"/>
       <c r="D10" s="84" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E10" s="94"/>
       <c r="F10" s="94"/>
@@ -10970,8 +10955,8 @@
       <c r="I10" s="84">
         <v>1</v>
       </c>
-      <c r="J10" s="130"/>
-      <c r="K10" s="131"/>
+      <c r="J10" s="142"/>
+      <c r="K10" s="143"/>
       <c r="L10" s="73"/>
       <c r="M10" s="73"/>
       <c r="N10" s="73"/>
@@ -10983,12 +10968,12 @@
     </row>
     <row r="11" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B11" s="80"/>
       <c r="C11" s="80"/>
       <c r="D11" s="84" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E11" s="94"/>
       <c r="F11" s="94"/>
@@ -10997,8 +10982,8 @@
       <c r="I11" s="84">
         <v>1</v>
       </c>
-      <c r="J11" s="130"/>
-      <c r="K11" s="131"/>
+      <c r="J11" s="142"/>
+      <c r="K11" s="143"/>
       <c r="L11" s="73"/>
       <c r="M11" s="73"/>
       <c r="N11" s="73"/>
@@ -11010,12 +10995,12 @@
     </row>
     <row r="12" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B12" s="80"/>
       <c r="C12" s="80"/>
       <c r="D12" s="84" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E12" s="94"/>
       <c r="F12" s="94"/>
@@ -11024,8 +11009,8 @@
       <c r="I12" s="84">
         <v>1</v>
       </c>
-      <c r="J12" s="130"/>
-      <c r="K12" s="131"/>
+      <c r="J12" s="142"/>
+      <c r="K12" s="143"/>
       <c r="L12" s="73"/>
       <c r="M12" s="73"/>
       <c r="N12" s="73"/>
@@ -11037,22 +11022,22 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="90" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="90">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" s="97" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D13" s="98"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="90"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="90"/>
-      <c r="I13" s="90"/>
-      <c r="J13" s="130"/>
-      <c r="K13" s="131"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="98"/>
+      <c r="G13" s="98"/>
+      <c r="H13" s="98"/>
+      <c r="I13" s="98"/>
+      <c r="J13" s="142"/>
+      <c r="K13" s="143"/>
       <c r="L13" s="73"/>
       <c r="M13" s="73"/>
       <c r="N13" s="73"/>
@@ -11062,30 +11047,24 @@
       <c r="R13" s="73"/>
       <c r="S13" s="73"/>
     </row>
-    <row r="14" spans="1:19" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
+    <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="75" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="86"/>
+      <c r="C14" s="84"/>
       <c r="D14" s="84" t="s">
-        <v>143</v>
-      </c>
-      <c r="E14" s="96">
-        <v>3</v>
-      </c>
-      <c r="F14" s="96">
+        <v>138</v>
+      </c>
+      <c r="E14" s="92">
         <v>2</v>
       </c>
-      <c r="G14" s="96">
-        <v>4</v>
-      </c>
-      <c r="H14" s="84">
-        <v>5</v>
-      </c>
-      <c r="I14" s="80"/>
-      <c r="J14" s="130"/>
-      <c r="K14" s="131"/>
+      <c r="F14" s="95"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
+      <c r="J14" s="142"/>
+      <c r="K14" s="143"/>
       <c r="L14" s="73"/>
       <c r="M14" s="73"/>
       <c r="N14" s="73"/>
@@ -11096,21 +11075,25 @@
       <c r="S14" s="73"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="36" t="s">
-        <v>78</v>
+      <c r="A15" s="80" t="s">
+        <v>134</v>
       </c>
       <c r="B15" s="80"/>
-      <c r="C15" s="80"/>
+      <c r="C15" s="84"/>
       <c r="D15" s="84" t="s">
-        <v>143</v>
-      </c>
-      <c r="E15" s="94"/>
-      <c r="F15" s="94"/>
+        <v>138</v>
+      </c>
+      <c r="E15" s="96">
+        <v>1</v>
+      </c>
+      <c r="F15" s="95">
+        <v>2</v>
+      </c>
       <c r="G15" s="94"/>
-      <c r="H15" s="80"/>
-      <c r="I15" s="80"/>
-      <c r="J15" s="130"/>
-      <c r="K15" s="131"/>
+      <c r="H15" s="94"/>
+      <c r="I15" s="94"/>
+      <c r="J15" s="142"/>
+      <c r="K15" s="143"/>
       <c r="L15" s="73"/>
       <c r="M15" s="73"/>
       <c r="N15" s="73"/>
@@ -11121,23 +11104,34 @@
       <c r="S15" s="73"/>
     </row>
     <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="90" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="90">
-        <v>2</v>
-      </c>
-      <c r="C16" s="97" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="98"/>
-      <c r="E16" s="90"/>
-      <c r="F16" s="90"/>
-      <c r="G16" s="90"/>
-      <c r="H16" s="90"/>
-      <c r="I16" s="90"/>
-      <c r="J16" s="130"/>
-      <c r="K16" s="131"/>
+      <c r="A16" s="87" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="87"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87">
+        <f>SUM(E4:E12)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="87">
+        <f>SUM(F3:F12)</f>
+        <v>1</v>
+      </c>
+      <c r="G16" s="87">
+        <f>SUM(G3:G12)</f>
+        <v>1</v>
+      </c>
+      <c r="H16" s="87">
+        <f>SUM(H3:H12)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="87">
+        <f>SUM(I3:I12)</f>
+        <v>14</v>
+      </c>
+      <c r="J16" s="144"/>
+      <c r="K16" s="145"/>
       <c r="L16" s="73"/>
       <c r="M16" s="73"/>
       <c r="N16" s="73"/>
@@ -11147,28 +11141,9 @@
       <c r="R16" s="73"/>
       <c r="S16" s="73"/>
     </row>
-    <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" s="80"/>
-      <c r="D17" s="84" t="s">
-        <v>143</v>
-      </c>
-      <c r="E17" s="3">
-        <v>3</v>
-      </c>
-      <c r="F17" s="3">
-        <v>4</v>
-      </c>
-      <c r="G17" s="3">
-        <v>1</v>
-      </c>
-      <c r="H17" s="3">
-        <v>2</v>
-      </c>
-      <c r="J17" s="130"/>
-      <c r="K17" s="131"/>
+    <row r="17" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
       <c r="L17" s="73"/>
       <c r="M17" s="73"/>
       <c r="N17" s="73"/>
@@ -11178,16 +11153,9 @@
       <c r="R17" s="73"/>
       <c r="S17" s="73"/>
     </row>
-    <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="80"/>
-      <c r="D18" s="84" t="s">
-        <v>143</v>
-      </c>
-      <c r="J18" s="130"/>
-      <c r="K18" s="131"/>
+    <row r="18" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="73"/>
+      <c r="K18" s="73"/>
       <c r="L18" s="73"/>
       <c r="M18" s="73"/>
       <c r="N18" s="73"/>
@@ -11197,24 +11165,9 @@
       <c r="R18" s="73"/>
       <c r="S18" s="73"/>
     </row>
-    <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="90">
-        <v>3</v>
-      </c>
-      <c r="C19" s="97" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="98"/>
-      <c r="E19" s="98"/>
-      <c r="F19" s="98"/>
-      <c r="G19" s="98"/>
-      <c r="H19" s="98"/>
-      <c r="I19" s="98"/>
-      <c r="J19" s="130"/>
-      <c r="K19" s="131"/>
+    <row r="19" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J19" s="73"/>
+      <c r="K19" s="73"/>
       <c r="L19" s="73"/>
       <c r="M19" s="73"/>
       <c r="N19" s="73"/>
@@ -11224,24 +11177,9 @@
       <c r="R19" s="73"/>
       <c r="S19" s="73"/>
     </row>
-    <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="75" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="86"/>
-      <c r="C20" s="84"/>
-      <c r="D20" s="84" t="s">
-        <v>143</v>
-      </c>
-      <c r="E20" s="92">
-        <v>2</v>
-      </c>
-      <c r="F20" s="95"/>
-      <c r="G20" s="86"/>
-      <c r="H20" s="86"/>
-      <c r="I20" s="86"/>
-      <c r="J20" s="130"/>
-      <c r="K20" s="131"/>
+    <row r="20" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J20" s="73"/>
+      <c r="K20" s="73"/>
       <c r="L20" s="73"/>
       <c r="M20" s="73"/>
       <c r="N20" s="73"/>
@@ -11251,26 +11189,9 @@
       <c r="R20" s="73"/>
       <c r="S20" s="73"/>
     </row>
-    <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="80" t="s">
-        <v>139</v>
-      </c>
-      <c r="B21" s="80"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="84" t="s">
-        <v>143</v>
-      </c>
-      <c r="E21" s="96">
-        <v>1</v>
-      </c>
-      <c r="F21" s="95">
-        <v>2</v>
-      </c>
-      <c r="G21" s="94"/>
-      <c r="H21" s="94"/>
-      <c r="I21" s="94"/>
-      <c r="J21" s="130"/>
-      <c r="K21" s="131"/>
+    <row r="21" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J21" s="73"/>
+      <c r="K21" s="73"/>
       <c r="L21" s="73"/>
       <c r="M21" s="73"/>
       <c r="N21" s="73"/>
@@ -11280,35 +11201,9 @@
       <c r="R21" s="73"/>
       <c r="S21" s="73"/>
     </row>
-    <row r="22" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="87" t="s">
-        <v>136</v>
-      </c>
-      <c r="B22" s="87"/>
-      <c r="C22" s="87"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="87">
-        <f>SUM(E4:E18)</f>
-        <v>6</v>
-      </c>
-      <c r="F22" s="87">
-        <f t="shared" ref="F22:I22" si="0">SUM(F3:F18)</f>
-        <v>7</v>
-      </c>
-      <c r="G22" s="87">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H22" s="87">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="I22" s="87">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="J22" s="132"/>
-      <c r="K22" s="133"/>
+    <row r="22" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J22" s="73"/>
+      <c r="K22" s="73"/>
       <c r="L22" s="73"/>
       <c r="M22" s="73"/>
       <c r="N22" s="73"/>
@@ -11318,7 +11213,7 @@
       <c r="R22" s="73"/>
       <c r="S22" s="73"/>
     </row>
-    <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J23" s="73"/>
       <c r="K23" s="73"/>
       <c r="L23" s="73"/>
@@ -11330,7 +11225,7 @@
       <c r="R23" s="73"/>
       <c r="S23" s="73"/>
     </row>
-    <row r="24" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J24" s="73"/>
       <c r="K24" s="73"/>
       <c r="L24" s="73"/>
@@ -11342,7 +11237,7 @@
       <c r="R24" s="73"/>
       <c r="S24" s="73"/>
     </row>
-    <row r="25" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J25" s="73"/>
       <c r="K25" s="73"/>
       <c r="L25" s="73"/>
@@ -11354,7 +11249,7 @@
       <c r="R25" s="73"/>
       <c r="S25" s="73"/>
     </row>
-    <row r="26" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J26" s="73"/>
       <c r="K26" s="73"/>
       <c r="L26" s="73"/>
@@ -11366,7 +11261,7 @@
       <c r="R26" s="73"/>
       <c r="S26" s="73"/>
     </row>
-    <row r="27" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J27" s="73"/>
       <c r="K27" s="73"/>
       <c r="L27" s="73"/>
@@ -11378,7 +11273,7 @@
       <c r="R27" s="73"/>
       <c r="S27" s="73"/>
     </row>
-    <row r="28" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J28" s="73"/>
       <c r="K28" s="73"/>
       <c r="L28" s="73"/>
@@ -11390,7 +11285,7 @@
       <c r="R28" s="73"/>
       <c r="S28" s="73"/>
     </row>
-    <row r="29" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J29" s="73"/>
       <c r="K29" s="73"/>
       <c r="L29" s="73"/>
@@ -11402,91 +11297,25 @@
       <c r="R29" s="73"/>
       <c r="S29" s="73"/>
     </row>
-    <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J30" s="73"/>
-      <c r="K30" s="73"/>
-      <c r="L30" s="73"/>
-      <c r="M30" s="73"/>
-      <c r="N30" s="73"/>
-      <c r="O30" s="73"/>
-      <c r="P30" s="73"/>
-      <c r="Q30" s="73"/>
-      <c r="R30" s="73"/>
-      <c r="S30" s="73"/>
-    </row>
-    <row r="31" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J31" s="73"/>
-      <c r="K31" s="73"/>
-      <c r="L31" s="73"/>
-      <c r="M31" s="73"/>
-      <c r="N31" s="73"/>
-      <c r="O31" s="73"/>
-      <c r="P31" s="73"/>
-      <c r="Q31" s="73"/>
-      <c r="R31" s="73"/>
-      <c r="S31" s="73"/>
-    </row>
-    <row r="32" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J32" s="73"/>
-      <c r="K32" s="73"/>
-      <c r="L32" s="73"/>
-      <c r="M32" s="73"/>
-      <c r="N32" s="73"/>
-      <c r="O32" s="73"/>
-      <c r="P32" s="73"/>
-      <c r="Q32" s="73"/>
-      <c r="R32" s="73"/>
-      <c r="S32" s="73"/>
-    </row>
-    <row r="33" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J33" s="73"/>
-      <c r="K33" s="73"/>
-      <c r="L33" s="73"/>
-      <c r="M33" s="73"/>
-      <c r="N33" s="73"/>
-      <c r="O33" s="73"/>
-      <c r="P33" s="73"/>
-      <c r="Q33" s="73"/>
-      <c r="R33" s="73"/>
-      <c r="S33" s="73"/>
-    </row>
-    <row r="34" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J34" s="73"/>
-      <c r="K34" s="73"/>
-      <c r="L34" s="73"/>
-      <c r="M34" s="73"/>
-      <c r="N34" s="73"/>
-      <c r="O34" s="73"/>
-      <c r="P34" s="73"/>
-      <c r="Q34" s="73"/>
-      <c r="R34" s="73"/>
-      <c r="S34" s="73"/>
-    </row>
-    <row r="35" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J35" s="73"/>
-      <c r="K35" s="73"/>
-      <c r="L35" s="73"/>
-      <c r="M35" s="73"/>
-      <c r="N35" s="73"/>
-      <c r="O35" s="73"/>
-      <c r="P35" s="73"/>
-      <c r="Q35" s="73"/>
-      <c r="R35" s="73"/>
-      <c r="S35" s="73"/>
-    </row>
-    <row r="36" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12436,17 +12265,11 @@
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J3:K22"/>
+    <mergeCell ref="J3:K16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>